<commit_message>
Update Matriz Infraest. MinVivienda_15FEB2019_CDI-ICBF.xlsx
</commit_message>
<xml_diff>
--- a/Infraestructura/MinVivienda/Matriz Infraest. MinVivienda_15FEB2019_CDI-ICBF.xlsx
+++ b/Infraestructura/MinVivienda/Matriz Infraest. MinVivienda_15FEB2019_CDI-ICBF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmadrid/Documents/GitHub/Dotaciones2019/Infraestructura/MinVivienda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C974F4F8-FDA1-324B-8966-1F17B6ECB9F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219F8B47-9830-FF4C-95B6-E1306A289B48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="12300" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="64" r:id="rId1"/>
@@ -423,7 +423,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,18 +433,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,6 +448,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -654,14 +666,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,30 +704,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -731,39 +725,9 @@
     <xf numFmtId="42" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,10 +767,97 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="7" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -825,6 +876,7 @@
   <colors>
     <mruColors>
       <color rgb="FFFF66FF"/>
+      <color rgb="FFFF9300"/>
       <color rgb="FFCDACE6"/>
       <color rgb="FFA50021"/>
       <color rgb="FF000099"/>
@@ -1110,265 +1162,267 @@
   </sheetPr>
   <dimension ref="A2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="18" customWidth="1"/>
-    <col min="4" max="5" width="11.5" style="18"/>
-    <col min="6" max="7" width="14.83203125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="18"/>
-    <col min="10" max="10" width="15" style="18" customWidth="1"/>
-    <col min="11" max="12" width="11.5" style="18"/>
-    <col min="13" max="13" width="17.83203125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" style="18" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="18"/>
-    <col min="16" max="16" width="17.5" style="18" customWidth="1"/>
-    <col min="17" max="17" width="17.83203125" style="18" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" style="18" customWidth="1"/>
-    <col min="19" max="16384" width="11.5" style="18"/>
+    <col min="1" max="1" width="3" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="15"/>
+    <col min="5" max="5" width="0" style="15" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="15"/>
+    <col min="10" max="10" width="15" style="15" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="0" style="15" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="15" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="15"/>
+    <col min="16" max="16" width="17.5" style="15" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" style="15" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" style="15" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.5" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16" thickBot="1"/>
     <row r="3" spans="1:18" ht="37" thickBot="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="J3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="K3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="M3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="49" t="s">
+      <c r="O3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="50" t="s">
+      <c r="P3" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="50" t="s">
+      <c r="Q3" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="33.75" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="24">
         <v>200</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41">
+      <c r="G4" s="25"/>
+      <c r="H4" s="25">
         <v>65</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="44">
+      <c r="J4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="28">
         <v>0.7732</v>
       </c>
-      <c r="P4" s="45">
+      <c r="P4" s="29">
         <v>1544156155</v>
       </c>
-      <c r="Q4" s="46">
+      <c r="Q4" s="30">
         <v>0</v>
       </c>
-      <c r="R4" s="47">
+      <c r="R4" s="31">
         <v>1544156155</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="39.75" customHeight="1">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="39">
         <v>640</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="40">
         <v>940</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="40">
         <v>300</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="12">
+      <c r="J5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="43">
         <v>1</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="17">
         <v>10261842702</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <v>2600000000</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5" s="19">
         <v>12861842702</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="38">
         <v>4080</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="40">
         <v>940</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="40">
         <v>300</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="12">
+      <c r="J6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="43">
         <v>0.99</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="17">
         <v>10644341972</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="8">
         <v>2500000000</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="19">
         <v>13144341972</v>
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>1644</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1380,51 +1434,51 @@
       <c r="H7" s="1">
         <v>300</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="11">
         <v>1</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="17">
         <v>12294344231</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <v>0</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="19">
         <v>12294344231</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="30">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>1500</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1436,51 +1490,51 @@
       <c r="H8" s="1">
         <v>160</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" s="12">
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="11">
         <v>0.97</v>
       </c>
-      <c r="P8" s="23">
+      <c r="P8" s="17">
         <v>15209334302</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="8">
         <v>0</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="19">
         <v>18804563575</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="30">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>768</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1492,51 +1546,51 @@
       <c r="H9" s="1">
         <v>300</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O9" s="12">
+      <c r="J9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="11">
         <v>0.2777</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="17">
         <v>13510661991</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <v>583622732</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="19">
         <v>14094284723</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="36">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>984</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1546,105 +1600,105 @@
       <c r="H10" s="1">
         <v>300</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="12">
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="11">
         <v>1</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="17">
         <v>3456165437</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="8">
         <v>0</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="19">
         <v>3891707526</v>
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>1140</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
         <v>428</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="13" t="s">
+      <c r="N11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="10">
         <v>1</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="17">
         <v>3206883763</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="9">
         <v>0</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11" s="19">
         <v>3206883763</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="50.25" customHeight="1">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>4000</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1656,163 +1710,163 @@
       <c r="H12" s="1">
         <v>300</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="L12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O12" s="15">
+      <c r="N12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="13">
         <v>1</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="17">
         <v>12366683867</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="8">
         <v>0</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="19">
         <v>12366683867</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="36">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="39">
         <v>1122</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="40">
         <v>940</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="40">
         <v>300</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="15">
+      <c r="J13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="44">
         <v>0</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="17">
         <v>11032041589</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <v>3200000000</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="19">
         <v>14232041589</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="45">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="40">
         <v>900</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="40">
         <v>940</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="40">
         <v>300</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O14" s="12">
+      <c r="J14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14" s="43">
         <v>0.95</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="17">
         <v>12646888334</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="8">
         <v>0</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="19">
         <v>12646888334</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="30">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>1209</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1822,51 +1876,51 @@
       <c r="H15" s="1">
         <v>300</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="16">
+      <c r="J15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="14">
         <v>0.46929999999999999</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="17">
         <v>4334884994</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="8">
         <v>0</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="19">
         <v>4334884994</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>1348</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1876,51 +1930,51 @@
       <c r="H16" s="1">
         <v>300</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="12">
+      <c r="J16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="11">
         <v>0.996</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="17">
         <v>3535515339</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q16" s="8">
         <v>1238697659</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="19">
         <v>4774212998</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="30">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>810</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1932,51 +1986,51 @@
       <c r="H17" s="1">
         <v>65</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="12">
+      <c r="J17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="11">
         <v>0.69469999999999998</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P17" s="17">
         <v>10256716382.24</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="8">
         <v>0</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="19">
         <v>10256716382.24</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="45">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>1000</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1988,360 +2042,360 @@
       <c r="H18" s="1">
         <v>300</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O18" s="12">
+      <c r="K18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="11">
         <v>1</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="17">
         <v>11430977616</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="8">
         <v>1000000000</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="19">
         <v>12430977616</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:18" s="47" customFormat="1">
+      <c r="A19" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="53">
         <v>608</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="54">
         <v>940</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="54">
         <v>300</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O19" s="12">
+      <c r="J19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" s="56">
         <v>0</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="17">
         <v>13000000000</v>
       </c>
       <c r="Q19" s="9">
         <v>0</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="46">
         <v>13000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:18" s="47" customFormat="1">
+      <c r="A20" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="53">
         <v>718</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1">
+      <c r="G20" s="54"/>
+      <c r="H20" s="54">
         <v>300</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20" s="12">
+      <c r="J20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" s="56">
         <v>0</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="17">
         <v>4000000000</v>
       </c>
       <c r="Q20" s="9">
         <v>0</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="46">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="24" t="s">
+    <row r="21" spans="1:18" s="47" customFormat="1">
+      <c r="A21" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="53">
         <v>1080</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1">
+      <c r="G21" s="54"/>
+      <c r="H21" s="54">
         <v>300</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O21" s="12">
+      <c r="J21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" s="56">
         <v>0</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="17">
         <v>4000000000</v>
       </c>
       <c r="Q21" s="9">
         <v>0</v>
       </c>
-      <c r="R21" s="25">
+      <c r="R21" s="46">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:18" s="47" customFormat="1">
+      <c r="A22" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="53">
         <v>780</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1">
+      <c r="G22" s="54"/>
+      <c r="H22" s="54">
         <v>300</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O22" s="12">
+      <c r="J22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="56">
         <v>0</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="17">
         <v>4000000000</v>
       </c>
       <c r="Q22" s="9">
         <v>0</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22" s="46">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="24">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:18" s="47" customFormat="1" ht="24">
+      <c r="A23" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="53">
         <v>481</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1">
+      <c r="G23" s="54"/>
+      <c r="H23" s="54">
         <v>300</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O23" s="12">
+      <c r="J23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="56">
         <v>0</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="17">
         <v>4000000000</v>
       </c>
       <c r="Q23" s="9">
         <v>0</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23" s="46">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16" thickBot="1">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:18" s="47" customFormat="1" ht="16" thickBot="1">
+      <c r="A24" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="60">
         <v>715</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30">
+      <c r="G24" s="61"/>
+      <c r="H24" s="61">
         <v>300</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="N24" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="O24" s="33">
+      <c r="J24" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" s="63">
         <v>0</v>
       </c>
-      <c r="P24" s="34">
+      <c r="P24" s="20">
         <v>4000000000</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="48">
         <v>0</v>
       </c>
-      <c r="R24" s="36">
+      <c r="R24" s="49">
         <v>4000000000</v>
       </c>
     </row>

</xml_diff>